<commit_message>
Bill delete bug fix
</commit_message>
<xml_diff>
--- a/sorted_aging_report.xlsx
+++ b/sorted_aging_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O696"/>
+  <dimension ref="A1:O693"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,7 +633,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023-08-18</t>
+          <t>2024-01-16</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L4" t="n">
         <v>14999.17</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>14999.17</v>
+        <v>15999.17</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -9336,10 +9336,10 @@
         <v>0</v>
       </c>
       <c r="G162" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H162" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I162" t="n">
         <v>0</v>
@@ -9354,10 +9354,10 @@
         <v>0</v>
       </c>
       <c r="M162" t="n">
-        <v>165</v>
+        <v>265</v>
       </c>
       <c r="N162" t="n">
-        <v>165</v>
+        <v>465</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -10207,10 +10207,10 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>38420</v>
+        <v>238420</v>
       </c>
       <c r="E178" t="n">
-        <v>38420</v>
+        <v>238420</v>
       </c>
       <c r="F178" t="n">
         <v>0</v>
@@ -10237,7 +10237,7 @@
         <v>0</v>
       </c>
       <c r="N178" t="n">
-        <v>38420</v>
+        <v>238420</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -13177,7 +13177,7 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="E232" t="n">
         <v>0</v>
@@ -13189,7 +13189,7 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="I232" t="n">
         <v>0</v>
@@ -13207,7 +13207,7 @@
         <v>0</v>
       </c>
       <c r="N232" t="n">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -34092,7 +34092,7 @@
         <v>0</v>
       </c>
       <c r="I612" t="n">
-        <v>8042.78</v>
+        <v>-8042.78</v>
       </c>
       <c r="J612" t="n">
         <v>0</v>
@@ -34107,7 +34107,7 @@
         <v>0</v>
       </c>
       <c r="N612" t="n">
-        <v>8042.78</v>
+        <v>-8042.78</v>
       </c>
       <c r="O612" t="inlineStr">
         <is>
@@ -34118,21 +34118,21 @@
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>SB/01386</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C613" t="inlineStr">
         <is>
-          <t>2023-09-28</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D613" t="n">
-        <v>6705.42</v>
+        <v>248694.86</v>
       </c>
       <c r="E613" t="n">
         <v>0</v>
@@ -34147,7 +34147,7 @@
         <v>0</v>
       </c>
       <c r="I613" t="n">
-        <v>6705.42</v>
+        <v>0</v>
       </c>
       <c r="J613" t="n">
         <v>0</v>
@@ -34159,14 +34159,14 @@
         <v>0</v>
       </c>
       <c r="M613" t="n">
-        <v>0</v>
+        <v>-241695.13</v>
       </c>
       <c r="N613" t="n">
-        <v>6705.42</v>
+        <v>-241695.13</v>
       </c>
       <c r="O613" t="inlineStr">
         <is>
-          <t xml:space="preserve">2491 </t>
+          <t xml:space="preserve">L-000056 </t>
         </is>
       </c>
     </row>
@@ -34187,7 +34187,7 @@
         </is>
       </c>
       <c r="D614" t="n">
-        <v>248694.86</v>
+        <v>6000</v>
       </c>
       <c r="E614" t="n">
         <v>0</v>
@@ -34214,35 +34214,35 @@
         <v>0</v>
       </c>
       <c r="M614" t="n">
-        <v>-241695.13</v>
+        <v>6000</v>
       </c>
       <c r="N614" t="n">
-        <v>-241695.13</v>
+        <v>6000</v>
       </c>
       <c r="O614" t="inlineStr">
         <is>
-          <t xml:space="preserve">L-000056 </t>
+          <t xml:space="preserve">1858 </t>
         </is>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01422</t>
         </is>
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-09-29</t>
         </is>
       </c>
       <c r="D615" t="n">
-        <v>6000</v>
+        <v>452000</v>
       </c>
       <c r="E615" t="n">
         <v>0</v>
@@ -34257,7 +34257,7 @@
         <v>0</v>
       </c>
       <c r="I615" t="n">
-        <v>0</v>
+        <v>452000</v>
       </c>
       <c r="J615" t="n">
         <v>0</v>
@@ -34269,10 +34269,10 @@
         <v>0</v>
       </c>
       <c r="M615" t="n">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="N615" t="n">
-        <v>6000</v>
+        <v>452000</v>
       </c>
       <c r="O615" t="inlineStr">
         <is>
@@ -34283,21 +34283,21 @@
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>SB/01422</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C616" t="inlineStr">
         <is>
-          <t>2023-09-29</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D616" t="n">
-        <v>452000</v>
+        <v>1893.5</v>
       </c>
       <c r="E616" t="n">
         <v>0</v>
@@ -34312,7 +34312,7 @@
         <v>0</v>
       </c>
       <c r="I616" t="n">
-        <v>452000</v>
+        <v>0</v>
       </c>
       <c r="J616" t="n">
         <v>0</v>
@@ -34324,38 +34324,38 @@
         <v>0</v>
       </c>
       <c r="M616" t="n">
-        <v>0</v>
+        <v>1893.5</v>
       </c>
       <c r="N616" t="n">
-        <v>452000</v>
+        <v>1893.5</v>
       </c>
       <c r="O616" t="inlineStr">
         <is>
-          <t xml:space="preserve">1858 </t>
+          <t xml:space="preserve">377 </t>
         </is>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>SB/02342</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>2023-11-24</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D617" t="n">
-        <v>339000</v>
+        <v>11.3</v>
       </c>
       <c r="E617" t="n">
-        <v>339000</v>
+        <v>0</v>
       </c>
       <c r="F617" t="n">
         <v>0</v>
@@ -34379,14 +34379,14 @@
         <v>0</v>
       </c>
       <c r="M617" t="n">
-        <v>0</v>
+        <v>-11.3</v>
       </c>
       <c r="N617" t="n">
-        <v>339000</v>
+        <v>-11.3</v>
       </c>
       <c r="O617" t="inlineStr">
         <is>
-          <t xml:space="preserve">1858 </t>
+          <t xml:space="preserve">1946 </t>
         </is>
       </c>
     </row>
@@ -34407,7 +34407,7 @@
         </is>
       </c>
       <c r="D618" t="n">
-        <v>1893.5</v>
+        <v>31.33</v>
       </c>
       <c r="E618" t="n">
         <v>0</v>
@@ -34434,35 +34434,35 @@
         <v>0</v>
       </c>
       <c r="M618" t="n">
-        <v>1893.5</v>
+        <v>31.33</v>
       </c>
       <c r="N618" t="n">
-        <v>1893.5</v>
+        <v>31.33</v>
       </c>
       <c r="O618" t="inlineStr">
         <is>
-          <t xml:space="preserve">377 </t>
+          <t xml:space="preserve">2161 </t>
         </is>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00392</t>
         </is>
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-07</t>
         </is>
       </c>
       <c r="D619" t="n">
-        <v>11.3</v>
+        <v>248600</v>
       </c>
       <c r="E619" t="n">
         <v>0</v>
@@ -34489,35 +34489,35 @@
         <v>0</v>
       </c>
       <c r="M619" t="n">
-        <v>-11.3</v>
+        <v>248600</v>
       </c>
       <c r="N619" t="n">
-        <v>-11.3</v>
+        <v>248600</v>
       </c>
       <c r="O619" t="inlineStr">
         <is>
-          <t xml:space="preserve">1946 </t>
+          <t xml:space="preserve">2323 </t>
         </is>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01110</t>
         </is>
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-09-15</t>
         </is>
       </c>
       <c r="D620" t="n">
-        <v>31.33</v>
+        <v>124300</v>
       </c>
       <c r="E620" t="n">
         <v>0</v>
@@ -34535,7 +34535,7 @@
         <v>0</v>
       </c>
       <c r="J620" t="n">
-        <v>0</v>
+        <v>124300</v>
       </c>
       <c r="K620" t="n">
         <v>0</v>
@@ -34544,35 +34544,35 @@
         <v>0</v>
       </c>
       <c r="M620" t="n">
-        <v>31.33</v>
+        <v>0</v>
       </c>
       <c r="N620" t="n">
-        <v>31.33</v>
+        <v>124300</v>
       </c>
       <c r="O620" t="inlineStr">
         <is>
-          <t xml:space="preserve">2161 </t>
+          <t xml:space="preserve">2323 </t>
         </is>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>SB/00392</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C621" t="inlineStr">
         <is>
-          <t>2023-08-07</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D621" t="n">
-        <v>248600</v>
+        <v>0.36</v>
       </c>
       <c r="E621" t="n">
         <v>0</v>
@@ -34599,14 +34599,14 @@
         <v>0</v>
       </c>
       <c r="M621" t="n">
-        <v>248600</v>
+        <v>0.36</v>
       </c>
       <c r="N621" t="n">
-        <v>248600</v>
+        <v>0.36</v>
       </c>
       <c r="O621" t="inlineStr">
         <is>
-          <t xml:space="preserve">2323 </t>
+          <t xml:space="preserve">1045 </t>
         </is>
       </c>
     </row>
@@ -34618,16 +34618,16 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>SB/01110</t>
+          <t>SB/00204</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-07-27</t>
         </is>
       </c>
       <c r="D622" t="n">
-        <v>124300</v>
+        <v>4407</v>
       </c>
       <c r="E622" t="n">
         <v>0</v>
@@ -34645,7 +34645,7 @@
         <v>0</v>
       </c>
       <c r="J622" t="n">
-        <v>124300</v>
+        <v>0</v>
       </c>
       <c r="K622" t="n">
         <v>0</v>
@@ -34654,35 +34654,35 @@
         <v>0</v>
       </c>
       <c r="M622" t="n">
-        <v>0</v>
+        <v>4407</v>
       </c>
       <c r="N622" t="n">
-        <v>124300</v>
+        <v>4407</v>
       </c>
       <c r="O622" t="inlineStr">
         <is>
-          <t xml:space="preserve">2323 </t>
+          <t xml:space="preserve">2283 </t>
         </is>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00117</t>
         </is>
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="D623" t="n">
-        <v>0.36</v>
+        <v>1469</v>
       </c>
       <c r="E623" t="n">
         <v>0</v>
@@ -34709,14 +34709,14 @@
         <v>0</v>
       </c>
       <c r="M623" t="n">
-        <v>0.36</v>
+        <v>1469</v>
       </c>
       <c r="N623" t="n">
-        <v>0.36</v>
+        <v>1469</v>
       </c>
       <c r="O623" t="inlineStr">
         <is>
-          <t xml:space="preserve">1045 </t>
+          <t xml:space="preserve">2261 </t>
         </is>
       </c>
     </row>
@@ -34728,16 +34728,16 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>SB/00204</t>
+          <t>SB/01121</t>
         </is>
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>2023-09-15</t>
         </is>
       </c>
       <c r="D624" t="n">
-        <v>4407</v>
+        <v>3164</v>
       </c>
       <c r="E624" t="n">
         <v>0</v>
@@ -34755,7 +34755,7 @@
         <v>0</v>
       </c>
       <c r="J624" t="n">
-        <v>0</v>
+        <v>3164</v>
       </c>
       <c r="K624" t="n">
         <v>0</v>
@@ -34764,14 +34764,14 @@
         <v>0</v>
       </c>
       <c r="M624" t="n">
-        <v>4407</v>
+        <v>0</v>
       </c>
       <c r="N624" t="n">
-        <v>4407</v>
+        <v>3164</v>
       </c>
       <c r="O624" t="inlineStr">
         <is>
-          <t xml:space="preserve">2283 </t>
+          <t xml:space="preserve">170 </t>
         </is>
       </c>
     </row>
@@ -34783,22 +34783,22 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>SB/00117</t>
+          <t>SB/02205</t>
         </is>
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>2023-07-23</t>
+          <t>2023-11-16</t>
         </is>
       </c>
       <c r="D625" t="n">
-        <v>1469</v>
+        <v>5650</v>
       </c>
       <c r="E625" t="n">
         <v>0</v>
       </c>
       <c r="F625" t="n">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="G625" t="n">
         <v>0</v>
@@ -34819,35 +34819,35 @@
         <v>0</v>
       </c>
       <c r="M625" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="N625" t="n">
-        <v>1469</v>
+        <v>5650</v>
       </c>
       <c r="O625" t="inlineStr">
         <is>
-          <t xml:space="preserve">2261 </t>
+          <t xml:space="preserve">170 </t>
         </is>
       </c>
     </row>
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>SB/01121</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C626" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D626" t="n">
-        <v>3164</v>
+        <v>2236</v>
       </c>
       <c r="E626" t="n">
         <v>0</v>
@@ -34865,7 +34865,7 @@
         <v>0</v>
       </c>
       <c r="J626" t="n">
-        <v>3164</v>
+        <v>0</v>
       </c>
       <c r="K626" t="n">
         <v>0</v>
@@ -34874,14 +34874,14 @@
         <v>0</v>
       </c>
       <c r="M626" t="n">
-        <v>0</v>
+        <v>2236</v>
       </c>
       <c r="N626" t="n">
-        <v>3164</v>
+        <v>2236</v>
       </c>
       <c r="O626" t="inlineStr">
         <is>
-          <t xml:space="preserve">170 </t>
+          <t xml:space="preserve">340 </t>
         </is>
       </c>
     </row>
@@ -34893,22 +34893,22 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>SB/02205</t>
+          <t>SB/00535</t>
         </is>
       </c>
       <c r="C627" t="inlineStr">
         <is>
-          <t>2023-11-16</t>
+          <t>2023-08-15</t>
         </is>
       </c>
       <c r="D627" t="n">
-        <v>5650</v>
+        <v>49720</v>
       </c>
       <c r="E627" t="n">
         <v>0</v>
       </c>
       <c r="F627" t="n">
-        <v>5650</v>
+        <v>0</v>
       </c>
       <c r="G627" t="n">
         <v>0</v>
@@ -34926,38 +34926,38 @@
         <v>0</v>
       </c>
       <c r="L627" t="n">
-        <v>0</v>
+        <v>49720</v>
       </c>
       <c r="M627" t="n">
         <v>0</v>
       </c>
       <c r="N627" t="n">
-        <v>5650</v>
+        <v>49720</v>
       </c>
       <c r="O627" t="inlineStr">
         <is>
-          <t xml:space="preserve">170 </t>
+          <t xml:space="preserve">340 </t>
         </is>
       </c>
     </row>
     <row r="628">
       <c r="A628" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00837</t>
         </is>
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-30</t>
         </is>
       </c>
       <c r="D628" t="n">
-        <v>2236</v>
+        <v>122040</v>
       </c>
       <c r="E628" t="n">
         <v>0</v>
@@ -34978,16 +34978,16 @@
         <v>0</v>
       </c>
       <c r="K628" t="n">
-        <v>0</v>
+        <v>122040</v>
       </c>
       <c r="L628" t="n">
         <v>0</v>
       </c>
       <c r="M628" t="n">
-        <v>2236</v>
+        <v>0</v>
       </c>
       <c r="N628" t="n">
-        <v>2236</v>
+        <v>122040</v>
       </c>
       <c r="O628" t="inlineStr">
         <is>
@@ -35003,19 +35003,19 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>SB/00535</t>
+          <t>SB/02386</t>
         </is>
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>2023-08-15</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="D629" t="n">
-        <v>49720</v>
+        <v>45200</v>
       </c>
       <c r="E629" t="n">
-        <v>0</v>
+        <v>45200</v>
       </c>
       <c r="F629" t="n">
         <v>0</v>
@@ -35036,13 +35036,13 @@
         <v>0</v>
       </c>
       <c r="L629" t="n">
-        <v>49720</v>
+        <v>0</v>
       </c>
       <c r="M629" t="n">
         <v>0</v>
       </c>
       <c r="N629" t="n">
-        <v>49720</v>
+        <v>45200</v>
       </c>
       <c r="O629" t="inlineStr">
         <is>
@@ -35058,16 +35058,16 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>SB/00837</t>
+          <t>SB/01891</t>
         </is>
       </c>
       <c r="C630" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
+          <t>2023-10-19</t>
         </is>
       </c>
       <c r="D630" t="n">
-        <v>122040</v>
+        <v>3990.03</v>
       </c>
       <c r="E630" t="n">
         <v>0</v>
@@ -35079,7 +35079,7 @@
         <v>0</v>
       </c>
       <c r="H630" t="n">
-        <v>0</v>
+        <v>3990.03</v>
       </c>
       <c r="I630" t="n">
         <v>0</v>
@@ -35088,7 +35088,7 @@
         <v>0</v>
       </c>
       <c r="K630" t="n">
-        <v>122040</v>
+        <v>0</v>
       </c>
       <c r="L630" t="n">
         <v>0</v>
@@ -35097,11 +35097,11 @@
         <v>0</v>
       </c>
       <c r="N630" t="n">
-        <v>122040</v>
+        <v>3990.03</v>
       </c>
       <c r="O630" t="inlineStr">
         <is>
-          <t xml:space="preserve">340 </t>
+          <t xml:space="preserve">597 </t>
         </is>
       </c>
     </row>
@@ -35113,25 +35113,25 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>SB/02386</t>
+          <t>SB/01950</t>
         </is>
       </c>
       <c r="C631" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-10-29</t>
         </is>
       </c>
       <c r="D631" t="n">
-        <v>45200</v>
+        <v>3350.45</v>
       </c>
       <c r="E631" t="n">
-        <v>45200</v>
+        <v>0</v>
       </c>
       <c r="F631" t="n">
         <v>0</v>
       </c>
       <c r="G631" t="n">
-        <v>0</v>
+        <v>3350.45</v>
       </c>
       <c r="H631" t="n">
         <v>0</v>
@@ -35152,32 +35152,32 @@
         <v>0</v>
       </c>
       <c r="N631" t="n">
-        <v>45200</v>
+        <v>3350.45</v>
       </c>
       <c r="O631" t="inlineStr">
         <is>
-          <t xml:space="preserve">340 </t>
+          <t xml:space="preserve">597 </t>
         </is>
       </c>
     </row>
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>SB/01891</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C632" t="inlineStr">
         <is>
-          <t>2023-10-19</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D632" t="n">
-        <v>3990.03</v>
+        <v>11.3</v>
       </c>
       <c r="E632" t="n">
         <v>0</v>
@@ -35189,7 +35189,7 @@
         <v>0</v>
       </c>
       <c r="H632" t="n">
-        <v>3990.03</v>
+        <v>0</v>
       </c>
       <c r="I632" t="n">
         <v>0</v>
@@ -35204,35 +35204,35 @@
         <v>0</v>
       </c>
       <c r="M632" t="n">
-        <v>0</v>
+        <v>-11.3</v>
       </c>
       <c r="N632" t="n">
-        <v>3990.03</v>
+        <v>-11.3</v>
       </c>
       <c r="O632" t="inlineStr">
         <is>
-          <t xml:space="preserve">597 </t>
+          <t xml:space="preserve">1924 </t>
         </is>
       </c>
     </row>
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>SB/01950</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>2023-10-29</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D633" t="n">
-        <v>3350.45</v>
+        <v>208694.73</v>
       </c>
       <c r="E633" t="n">
         <v>0</v>
@@ -35241,7 +35241,7 @@
         <v>0</v>
       </c>
       <c r="G633" t="n">
-        <v>3350.45</v>
+        <v>0</v>
       </c>
       <c r="H633" t="n">
         <v>0</v>
@@ -35259,14 +35259,14 @@
         <v>0</v>
       </c>
       <c r="M633" t="n">
-        <v>0</v>
+        <v>208694.73</v>
       </c>
       <c r="N633" t="n">
-        <v>3350.45</v>
+        <v>208694.73</v>
       </c>
       <c r="O633" t="inlineStr">
         <is>
-          <t xml:space="preserve">597 </t>
+          <t xml:space="preserve">898 </t>
         </is>
       </c>
     </row>
@@ -35287,7 +35287,7 @@
         </is>
       </c>
       <c r="D634" t="n">
-        <v>11.3</v>
+        <v>0.78</v>
       </c>
       <c r="E634" t="n">
         <v>0</v>
@@ -35314,35 +35314,35 @@
         <v>0</v>
       </c>
       <c r="M634" t="n">
-        <v>-11.3</v>
+        <v>200</v>
       </c>
       <c r="N634" t="n">
-        <v>-11.3</v>
+        <v>200</v>
       </c>
       <c r="O634" t="inlineStr">
         <is>
-          <t xml:space="preserve">1924 </t>
+          <t xml:space="preserve">911 </t>
         </is>
       </c>
     </row>
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01725</t>
         </is>
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-10-12</t>
         </is>
       </c>
       <c r="D635" t="n">
-        <v>208694.73</v>
+        <v>3390</v>
       </c>
       <c r="E635" t="n">
         <v>0</v>
@@ -35357,7 +35357,7 @@
         <v>0</v>
       </c>
       <c r="I635" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J635" t="n">
         <v>0</v>
@@ -35369,35 +35369,35 @@
         <v>0</v>
       </c>
       <c r="M635" t="n">
-        <v>208694.73</v>
+        <v>0</v>
       </c>
       <c r="N635" t="n">
-        <v>208694.73</v>
+        <v>1000</v>
       </c>
       <c r="O635" t="inlineStr">
         <is>
-          <t xml:space="preserve">898 </t>
+          <t xml:space="preserve">2566 </t>
         </is>
       </c>
     </row>
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00382</t>
         </is>
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-06</t>
         </is>
       </c>
       <c r="D636" t="n">
-        <v>0.78</v>
+        <v>10000.5</v>
       </c>
       <c r="E636" t="n">
         <v>0</v>
@@ -35424,14 +35424,14 @@
         <v>0</v>
       </c>
       <c r="M636" t="n">
-        <v>0.78</v>
+        <v>8330.57</v>
       </c>
       <c r="N636" t="n">
-        <v>0.78</v>
+        <v>8330.57</v>
       </c>
       <c r="O636" t="inlineStr">
         <is>
-          <t xml:space="preserve">911 </t>
+          <t xml:space="preserve">1107 </t>
         </is>
       </c>
     </row>
@@ -35443,16 +35443,16 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>SB/01067</t>
+          <t>SB/00577</t>
         </is>
       </c>
       <c r="C637" t="inlineStr">
         <is>
-          <t>2024-01-18</t>
+          <t>2023-08-16</t>
         </is>
       </c>
       <c r="D637" t="n">
-        <v>1000.39</v>
+        <v>8000.4</v>
       </c>
       <c r="E637" t="n">
         <v>0</v>
@@ -35470,23 +35470,23 @@
         <v>0</v>
       </c>
       <c r="J637" t="n">
-        <v>1000.39</v>
+        <v>0</v>
       </c>
       <c r="K637" t="n">
         <v>0</v>
       </c>
       <c r="L637" t="n">
-        <v>0</v>
+        <v>8000.4</v>
       </c>
       <c r="M637" t="n">
         <v>0</v>
       </c>
       <c r="N637" t="n">
-        <v>1000.39</v>
+        <v>8000.4</v>
       </c>
       <c r="O637" t="inlineStr">
         <is>
-          <t xml:space="preserve">911 </t>
+          <t xml:space="preserve">1107 </t>
         </is>
       </c>
     </row>
@@ -35498,16 +35498,16 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>SB/01725</t>
+          <t>SB/00584</t>
         </is>
       </c>
       <c r="C638" t="inlineStr">
         <is>
-          <t>2023-10-12</t>
+          <t>2023-08-17</t>
         </is>
       </c>
       <c r="D638" t="n">
-        <v>3390</v>
+        <v>8000.4</v>
       </c>
       <c r="E638" t="n">
         <v>0</v>
@@ -35519,7 +35519,7 @@
         <v>0</v>
       </c>
       <c r="H638" t="n">
-        <v>3390</v>
+        <v>0</v>
       </c>
       <c r="I638" t="n">
         <v>0</v>
@@ -35531,17 +35531,17 @@
         <v>0</v>
       </c>
       <c r="L638" t="n">
-        <v>0</v>
+        <v>8000.4</v>
       </c>
       <c r="M638" t="n">
         <v>0</v>
       </c>
       <c r="N638" t="n">
-        <v>3390</v>
+        <v>8000.4</v>
       </c>
       <c r="O638" t="inlineStr">
         <is>
-          <t xml:space="preserve">2566 </t>
+          <t xml:space="preserve">1107 </t>
         </is>
       </c>
     </row>
@@ -35553,16 +35553,16 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>SB/00382</t>
+          <t>SB/00639</t>
         </is>
       </c>
       <c r="C639" t="inlineStr">
         <is>
-          <t>2023-08-06</t>
+          <t>2023-08-20</t>
         </is>
       </c>
       <c r="D639" t="n">
-        <v>10000.5</v>
+        <v>15000.07</v>
       </c>
       <c r="E639" t="n">
         <v>0</v>
@@ -35586,13 +35586,13 @@
         <v>0</v>
       </c>
       <c r="L639" t="n">
-        <v>0</v>
+        <v>15000.07</v>
       </c>
       <c r="M639" t="n">
-        <v>8330.57</v>
+        <v>0</v>
       </c>
       <c r="N639" t="n">
-        <v>8330.57</v>
+        <v>15000.07</v>
       </c>
       <c r="O639" t="inlineStr">
         <is>
@@ -35608,16 +35608,16 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>SB/00577</t>
+          <t>SB/01123</t>
         </is>
       </c>
       <c r="C640" t="inlineStr">
         <is>
-          <t>2023-08-16</t>
+          <t>2023-09-15</t>
         </is>
       </c>
       <c r="D640" t="n">
-        <v>8000.4</v>
+        <v>10000.5</v>
       </c>
       <c r="E640" t="n">
         <v>0</v>
@@ -35635,19 +35635,19 @@
         <v>0</v>
       </c>
       <c r="J640" t="n">
-        <v>0</v>
+        <v>10000.5</v>
       </c>
       <c r="K640" t="n">
         <v>0</v>
       </c>
       <c r="L640" t="n">
-        <v>8000.4</v>
+        <v>0</v>
       </c>
       <c r="M640" t="n">
         <v>0</v>
       </c>
       <c r="N640" t="n">
-        <v>8000.4</v>
+        <v>10000.5</v>
       </c>
       <c r="O640" t="inlineStr">
         <is>
@@ -35663,16 +35663,16 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>SB/00584</t>
+          <t>SB/01159</t>
         </is>
       </c>
       <c r="C641" t="inlineStr">
         <is>
-          <t>2023-08-17</t>
+          <t>2023-09-17</t>
         </is>
       </c>
       <c r="D641" t="n">
-        <v>8000.4</v>
+        <v>20001</v>
       </c>
       <c r="E641" t="n">
         <v>0</v>
@@ -35690,19 +35690,19 @@
         <v>0</v>
       </c>
       <c r="J641" t="n">
-        <v>0</v>
+        <v>20001</v>
       </c>
       <c r="K641" t="n">
         <v>0</v>
       </c>
       <c r="L641" t="n">
-        <v>8000.4</v>
+        <v>0</v>
       </c>
       <c r="M641" t="n">
         <v>0</v>
       </c>
       <c r="N641" t="n">
-        <v>8000.4</v>
+        <v>20001</v>
       </c>
       <c r="O641" t="inlineStr">
         <is>
@@ -35718,16 +35718,16 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>SB/00639</t>
+          <t>SB/01568</t>
         </is>
       </c>
       <c r="C642" t="inlineStr">
         <is>
-          <t>2023-08-20</t>
+          <t>2023-10-05</t>
         </is>
       </c>
       <c r="D642" t="n">
-        <v>15000.07</v>
+        <v>5000.93</v>
       </c>
       <c r="E642" t="n">
         <v>0</v>
@@ -35742,7 +35742,7 @@
         <v>0</v>
       </c>
       <c r="I642" t="n">
-        <v>0</v>
+        <v>5000.93</v>
       </c>
       <c r="J642" t="n">
         <v>0</v>
@@ -35751,13 +35751,13 @@
         <v>0</v>
       </c>
       <c r="L642" t="n">
-        <v>15000.07</v>
+        <v>0</v>
       </c>
       <c r="M642" t="n">
         <v>0</v>
       </c>
       <c r="N642" t="n">
-        <v>15000.07</v>
+        <v>5000.93</v>
       </c>
       <c r="O642" t="inlineStr">
         <is>
@@ -35773,16 +35773,16 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>SB/01123</t>
+          <t>SB/01839</t>
         </is>
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-10-17</t>
         </is>
       </c>
       <c r="D643" t="n">
-        <v>10000.5</v>
+        <v>7000.35</v>
       </c>
       <c r="E643" t="n">
         <v>0</v>
@@ -35794,13 +35794,13 @@
         <v>0</v>
       </c>
       <c r="H643" t="n">
-        <v>0</v>
+        <v>7000.35</v>
       </c>
       <c r="I643" t="n">
         <v>0</v>
       </c>
       <c r="J643" t="n">
-        <v>10000.5</v>
+        <v>0</v>
       </c>
       <c r="K643" t="n">
         <v>0</v>
@@ -35812,7 +35812,7 @@
         <v>0</v>
       </c>
       <c r="N643" t="n">
-        <v>10000.5</v>
+        <v>7000.35</v>
       </c>
       <c r="O643" t="inlineStr">
         <is>
@@ -35828,16 +35828,16 @@
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>SB/01159</t>
+          <t>SB/01962</t>
         </is>
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>2023-09-17</t>
+          <t>2023-10-29</t>
         </is>
       </c>
       <c r="D644" t="n">
-        <v>20001</v>
+        <v>8001.76</v>
       </c>
       <c r="E644" t="n">
         <v>0</v>
@@ -35846,7 +35846,7 @@
         <v>0</v>
       </c>
       <c r="G644" t="n">
-        <v>0</v>
+        <v>8001.76</v>
       </c>
       <c r="H644" t="n">
         <v>0</v>
@@ -35855,7 +35855,7 @@
         <v>0</v>
       </c>
       <c r="J644" t="n">
-        <v>20001</v>
+        <v>0</v>
       </c>
       <c r="K644" t="n">
         <v>0</v>
@@ -35867,7 +35867,7 @@
         <v>0</v>
       </c>
       <c r="N644" t="n">
-        <v>20001</v>
+        <v>8001.76</v>
       </c>
       <c r="O644" t="inlineStr">
         <is>
@@ -35883,16 +35883,16 @@
       </c>
       <c r="B645" t="inlineStr">
         <is>
-          <t>SB/01568</t>
+          <t>SB/01963</t>
         </is>
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>2023-10-05</t>
+          <t>2023-10-29</t>
         </is>
       </c>
       <c r="D645" t="n">
-        <v>5000.93</v>
+        <v>18001.13</v>
       </c>
       <c r="E645" t="n">
         <v>0</v>
@@ -35901,13 +35901,13 @@
         <v>0</v>
       </c>
       <c r="G645" t="n">
-        <v>0</v>
+        <v>18001.13</v>
       </c>
       <c r="H645" t="n">
         <v>0</v>
       </c>
       <c r="I645" t="n">
-        <v>5000.93</v>
+        <v>0</v>
       </c>
       <c r="J645" t="n">
         <v>0</v>
@@ -35922,7 +35922,7 @@
         <v>0</v>
       </c>
       <c r="N645" t="n">
-        <v>5000.93</v>
+        <v>18001.13</v>
       </c>
       <c r="O645" t="inlineStr">
         <is>
@@ -35938,28 +35938,28 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>SB/01839</t>
+          <t>SB/02213</t>
         </is>
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>2023-10-17</t>
+          <t>2023-11-16</t>
         </is>
       </c>
       <c r="D646" t="n">
-        <v>7000.35</v>
+        <v>5999.96</v>
       </c>
       <c r="E646" t="n">
         <v>0</v>
       </c>
       <c r="F646" t="n">
-        <v>0</v>
+        <v>5999.96</v>
       </c>
       <c r="G646" t="n">
         <v>0</v>
       </c>
       <c r="H646" t="n">
-        <v>7000.35</v>
+        <v>0</v>
       </c>
       <c r="I646" t="n">
         <v>0</v>
@@ -35977,7 +35977,7 @@
         <v>0</v>
       </c>
       <c r="N646" t="n">
-        <v>7000.35</v>
+        <v>5999.96</v>
       </c>
       <c r="O646" t="inlineStr">
         <is>
@@ -35993,25 +35993,25 @@
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>SB/01962</t>
+          <t>SB/02370</t>
         </is>
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>2023-10-29</t>
+          <t>2023-11-26</t>
         </is>
       </c>
       <c r="D647" t="n">
-        <v>8001.76</v>
+        <v>8001.19</v>
       </c>
       <c r="E647" t="n">
-        <v>0</v>
+        <v>8001.19</v>
       </c>
       <c r="F647" t="n">
         <v>0</v>
       </c>
       <c r="G647" t="n">
-        <v>8001.76</v>
+        <v>0</v>
       </c>
       <c r="H647" t="n">
         <v>0</v>
@@ -36032,7 +36032,7 @@
         <v>0</v>
       </c>
       <c r="N647" t="n">
-        <v>8001.76</v>
+        <v>8001.19</v>
       </c>
       <c r="O647" t="inlineStr">
         <is>
@@ -36048,25 +36048,25 @@
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>SB/01963</t>
+          <t>SB/02395</t>
         </is>
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>2023-10-29</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="D648" t="n">
-        <v>18001.13</v>
+        <v>9999.940000000001</v>
       </c>
       <c r="E648" t="n">
-        <v>0</v>
+        <v>9999.940000000001</v>
       </c>
       <c r="F648" t="n">
         <v>0</v>
       </c>
       <c r="G648" t="n">
-        <v>18001.13</v>
+        <v>0</v>
       </c>
       <c r="H648" t="n">
         <v>0</v>
@@ -36087,7 +36087,7 @@
         <v>0</v>
       </c>
       <c r="N648" t="n">
-        <v>18001.13</v>
+        <v>9999.940000000001</v>
       </c>
       <c r="O648" t="inlineStr">
         <is>
@@ -36103,22 +36103,22 @@
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>SB/02213</t>
+          <t>SB/00623</t>
         </is>
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>2023-11-16</t>
+          <t>2023-08-18</t>
         </is>
       </c>
       <c r="D649" t="n">
-        <v>5999.96</v>
+        <v>1469</v>
       </c>
       <c r="E649" t="n">
         <v>0</v>
       </c>
       <c r="F649" t="n">
-        <v>5999.96</v>
+        <v>0</v>
       </c>
       <c r="G649" t="n">
         <v>0</v>
@@ -36136,17 +36136,17 @@
         <v>0</v>
       </c>
       <c r="L649" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="M649" t="n">
         <v>0</v>
       </c>
       <c r="N649" t="n">
-        <v>5999.96</v>
+        <v>1469</v>
       </c>
       <c r="O649" t="inlineStr">
         <is>
-          <t xml:space="preserve">1107 </t>
+          <t xml:space="preserve">2375 </t>
         </is>
       </c>
     </row>
@@ -36158,19 +36158,19 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>SB/02370</t>
+          <t>SB/00888</t>
         </is>
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>2023-11-26</t>
+          <t>2023-09-03</t>
         </is>
       </c>
       <c r="D650" t="n">
-        <v>8001.19</v>
+        <v>1469</v>
       </c>
       <c r="E650" t="n">
-        <v>8001.19</v>
+        <v>0</v>
       </c>
       <c r="F650" t="n">
         <v>0</v>
@@ -36188,7 +36188,7 @@
         <v>0</v>
       </c>
       <c r="K650" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="L650" t="n">
         <v>0</v>
@@ -36197,11 +36197,11 @@
         <v>0</v>
       </c>
       <c r="N650" t="n">
-        <v>8001.19</v>
+        <v>1469</v>
       </c>
       <c r="O650" t="inlineStr">
         <is>
-          <t xml:space="preserve">1107 </t>
+          <t xml:space="preserve">2375 </t>
         </is>
       </c>
     </row>
@@ -36213,19 +36213,19 @@
       </c>
       <c r="B651" t="inlineStr">
         <is>
-          <t>SB/02395</t>
+          <t>SB/01037</t>
         </is>
       </c>
       <c r="C651" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-09-12</t>
         </is>
       </c>
       <c r="D651" t="n">
-        <v>9999.940000000001</v>
+        <v>1469</v>
       </c>
       <c r="E651" t="n">
-        <v>9999.940000000001</v>
+        <v>0</v>
       </c>
       <c r="F651" t="n">
         <v>0</v>
@@ -36240,7 +36240,7 @@
         <v>0</v>
       </c>
       <c r="J651" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="K651" t="n">
         <v>0</v>
@@ -36252,11 +36252,11 @@
         <v>0</v>
       </c>
       <c r="N651" t="n">
-        <v>9999.940000000001</v>
+        <v>1469</v>
       </c>
       <c r="O651" t="inlineStr">
         <is>
-          <t xml:space="preserve">1107 </t>
+          <t xml:space="preserve">2375 </t>
         </is>
       </c>
     </row>
@@ -36268,12 +36268,12 @@
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>SB/00623</t>
+          <t>SB/01243</t>
         </is>
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>2023-08-18</t>
+          <t>2023-09-21</t>
         </is>
       </c>
       <c r="D652" t="n">
@@ -36295,13 +36295,13 @@
         <v>0</v>
       </c>
       <c r="J652" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="K652" t="n">
         <v>0</v>
       </c>
       <c r="L652" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="M652" t="n">
         <v>0</v>
@@ -36323,12 +36323,12 @@
       </c>
       <c r="B653" t="inlineStr">
         <is>
-          <t>SB/00888</t>
+          <t>SB/01388</t>
         </is>
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>2023-09-03</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="D653" t="n">
@@ -36347,13 +36347,13 @@
         <v>0</v>
       </c>
       <c r="I653" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="J653" t="n">
         <v>0</v>
       </c>
       <c r="K653" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="L653" t="n">
         <v>0</v>
@@ -36378,12 +36378,12 @@
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>SB/01037</t>
+          <t>SB/01625</t>
         </is>
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>2023-09-12</t>
+          <t>2023-10-08</t>
         </is>
       </c>
       <c r="D654" t="n">
@@ -36399,13 +36399,13 @@
         <v>0</v>
       </c>
       <c r="H654" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="I654" t="n">
         <v>0</v>
       </c>
       <c r="J654" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="K654" t="n">
         <v>0</v>
@@ -36433,12 +36433,12 @@
       </c>
       <c r="B655" t="inlineStr">
         <is>
-          <t>SB/01243</t>
+          <t>SB/01729</t>
         </is>
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>2023-09-21</t>
+          <t>2023-10-12</t>
         </is>
       </c>
       <c r="D655" t="n">
@@ -36454,13 +36454,13 @@
         <v>0</v>
       </c>
       <c r="H655" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="I655" t="n">
         <v>0</v>
       </c>
       <c r="J655" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="K655" t="n">
         <v>0</v>
@@ -36483,21 +36483,21 @@
     <row r="656">
       <c r="A656" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B656" t="inlineStr">
         <is>
-          <t>SB/01388</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>2023-09-28</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D656" t="n">
-        <v>1469</v>
+        <v>45765</v>
       </c>
       <c r="E656" t="n">
         <v>0</v>
@@ -36512,7 +36512,7 @@
         <v>0</v>
       </c>
       <c r="I656" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="J656" t="n">
         <v>0</v>
@@ -36524,35 +36524,35 @@
         <v>0</v>
       </c>
       <c r="M656" t="n">
-        <v>0</v>
+        <v>-2542.5</v>
       </c>
       <c r="N656" t="n">
-        <v>1469</v>
+        <v>-2542.5</v>
       </c>
       <c r="O656" t="inlineStr">
         <is>
-          <t xml:space="preserve">2375 </t>
+          <t xml:space="preserve">253 </t>
         </is>
       </c>
     </row>
     <row r="657">
       <c r="A657" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B657" t="inlineStr">
         <is>
-          <t>SB/01625</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>2023-10-08</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D657" t="n">
-        <v>1469</v>
+        <v>0.11</v>
       </c>
       <c r="E657" t="n">
         <v>0</v>
@@ -36564,7 +36564,7 @@
         <v>0</v>
       </c>
       <c r="H657" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="I657" t="n">
         <v>0</v>
@@ -36579,35 +36579,35 @@
         <v>0</v>
       </c>
       <c r="M657" t="n">
-        <v>0</v>
+        <v>-0.11</v>
       </c>
       <c r="N657" t="n">
-        <v>1469</v>
+        <v>-0.11</v>
       </c>
       <c r="O657" t="inlineStr">
         <is>
-          <t xml:space="preserve">2375 </t>
+          <t xml:space="preserve">1955 </t>
         </is>
       </c>
     </row>
     <row r="658">
       <c r="A658" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B658" t="inlineStr">
         <is>
-          <t>SB/01729</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>2023-10-12</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D658" t="n">
-        <v>1469</v>
+        <v>0.5</v>
       </c>
       <c r="E658" t="n">
         <v>0</v>
@@ -36619,7 +36619,7 @@
         <v>0</v>
       </c>
       <c r="H658" t="n">
-        <v>1469</v>
+        <v>0</v>
       </c>
       <c r="I658" t="n">
         <v>0</v>
@@ -36634,35 +36634,35 @@
         <v>0</v>
       </c>
       <c r="M658" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N658" t="n">
-        <v>1469</v>
+        <v>0.5</v>
       </c>
       <c r="O658" t="inlineStr">
         <is>
-          <t xml:space="preserve">2375 </t>
+          <t xml:space="preserve">668 </t>
         </is>
       </c>
     </row>
     <row r="659">
       <c r="A659" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B659" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01363</t>
         </is>
       </c>
       <c r="C659" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-09-27</t>
         </is>
       </c>
       <c r="D659" t="n">
-        <v>45765</v>
+        <v>5650</v>
       </c>
       <c r="E659" t="n">
         <v>0</v>
@@ -36677,7 +36677,7 @@
         <v>0</v>
       </c>
       <c r="I659" t="n">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="J659" t="n">
         <v>0</v>
@@ -36689,14 +36689,14 @@
         <v>0</v>
       </c>
       <c r="M659" t="n">
-        <v>-2542.5</v>
+        <v>0</v>
       </c>
       <c r="N659" t="n">
-        <v>-2542.5</v>
+        <v>5650</v>
       </c>
       <c r="O659" t="inlineStr">
         <is>
-          <t xml:space="preserve">253 </t>
+          <t xml:space="preserve">668 </t>
         </is>
       </c>
     </row>
@@ -36717,7 +36717,7 @@
         </is>
       </c>
       <c r="D660" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E660" t="n">
         <v>0</v>
@@ -36744,14 +36744,14 @@
         <v>0</v>
       </c>
       <c r="M660" t="n">
-        <v>-0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N660" t="n">
-        <v>-0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="O660" t="inlineStr">
         <is>
-          <t xml:space="preserve">1955 </t>
+          <t xml:space="preserve">873 </t>
         </is>
       </c>
     </row>
@@ -36772,7 +36772,7 @@
         </is>
       </c>
       <c r="D661" t="n">
-        <v>0.5</v>
+        <v>204</v>
       </c>
       <c r="E661" t="n">
         <v>0</v>
@@ -36799,35 +36799,35 @@
         <v>0</v>
       </c>
       <c r="M661" t="n">
-        <v>0.5</v>
+        <v>-204</v>
       </c>
       <c r="N661" t="n">
-        <v>0.5</v>
+        <v>-204</v>
       </c>
       <c r="O661" t="inlineStr">
         <is>
-          <t xml:space="preserve">668 </t>
+          <t xml:space="preserve">641 </t>
         </is>
       </c>
     </row>
     <row r="662">
       <c r="A662" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B662" t="inlineStr">
         <is>
-          <t>SB/01363</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C662" t="inlineStr">
         <is>
-          <t>2023-09-27</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D662" t="n">
-        <v>5650</v>
+        <v>0.49</v>
       </c>
       <c r="E662" t="n">
         <v>0</v>
@@ -36842,7 +36842,7 @@
         <v>0</v>
       </c>
       <c r="I662" t="n">
-        <v>5650</v>
+        <v>0</v>
       </c>
       <c r="J662" t="n">
         <v>0</v>
@@ -36854,14 +36854,14 @@
         <v>0</v>
       </c>
       <c r="M662" t="n">
-        <v>0</v>
+        <v>-0.49</v>
       </c>
       <c r="N662" t="n">
-        <v>5650</v>
+        <v>-0.49</v>
       </c>
       <c r="O662" t="inlineStr">
         <is>
-          <t xml:space="preserve">668 </t>
+          <t xml:space="preserve">836 </t>
         </is>
       </c>
     </row>
@@ -36882,7 +36882,7 @@
         </is>
       </c>
       <c r="D663" t="n">
-        <v>0.07000000000000001</v>
+        <v>47034.67</v>
       </c>
       <c r="E663" t="n">
         <v>0</v>
@@ -36909,35 +36909,35 @@
         <v>0</v>
       </c>
       <c r="M663" t="n">
-        <v>0.07000000000000001</v>
+        <v>47034.67</v>
       </c>
       <c r="N663" t="n">
-        <v>0.07000000000000001</v>
+        <v>47034.67</v>
       </c>
       <c r="O663" t="inlineStr">
         <is>
-          <t xml:space="preserve">873 </t>
+          <t xml:space="preserve">149 </t>
         </is>
       </c>
     </row>
     <row r="664">
       <c r="A664" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B664" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01486</t>
         </is>
       </c>
       <c r="C664" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-10-03</t>
         </is>
       </c>
       <c r="D664" t="n">
-        <v>204</v>
+        <v>10000.05</v>
       </c>
       <c r="E664" t="n">
         <v>0</v>
@@ -36952,7 +36952,7 @@
         <v>0</v>
       </c>
       <c r="I664" t="n">
-        <v>0</v>
+        <v>10000.05</v>
       </c>
       <c r="J664" t="n">
         <v>0</v>
@@ -36964,35 +36964,35 @@
         <v>0</v>
       </c>
       <c r="M664" t="n">
-        <v>-204</v>
+        <v>0</v>
       </c>
       <c r="N664" t="n">
-        <v>-204</v>
+        <v>10000.05</v>
       </c>
       <c r="O664" t="inlineStr">
         <is>
-          <t xml:space="preserve">641 </t>
+          <t xml:space="preserve">149 </t>
         </is>
       </c>
     </row>
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01663</t>
         </is>
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-10-09</t>
         </is>
       </c>
       <c r="D665" t="n">
-        <v>0.49</v>
+        <v>10000.05</v>
       </c>
       <c r="E665" t="n">
         <v>0</v>
@@ -37004,7 +37004,7 @@
         <v>0</v>
       </c>
       <c r="H665" t="n">
-        <v>0</v>
+        <v>10000.05</v>
       </c>
       <c r="I665" t="n">
         <v>0</v>
@@ -37019,35 +37019,35 @@
         <v>0</v>
       </c>
       <c r="M665" t="n">
-        <v>-0.49</v>
+        <v>0</v>
       </c>
       <c r="N665" t="n">
-        <v>-0.49</v>
+        <v>10000.05</v>
       </c>
       <c r="O665" t="inlineStr">
         <is>
-          <t xml:space="preserve">836 </t>
+          <t xml:space="preserve">149 </t>
         </is>
       </c>
     </row>
     <row r="666">
       <c r="A666" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00441</t>
         </is>
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-09</t>
         </is>
       </c>
       <c r="D666" t="n">
-        <v>47034.67</v>
+        <v>3955</v>
       </c>
       <c r="E666" t="n">
         <v>0</v>
@@ -37071,38 +37071,38 @@
         <v>0</v>
       </c>
       <c r="L666" t="n">
-        <v>0</v>
+        <v>3955</v>
       </c>
       <c r="M666" t="n">
-        <v>47034.67</v>
+        <v>0</v>
       </c>
       <c r="N666" t="n">
-        <v>47034.67</v>
+        <v>3955</v>
       </c>
       <c r="O666" t="inlineStr">
         <is>
-          <t xml:space="preserve">149 </t>
+          <t xml:space="preserve">2338 </t>
         </is>
       </c>
     </row>
     <row r="667">
       <c r="A667" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B667" t="inlineStr">
         <is>
-          <t>SB/01486</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C667" t="inlineStr">
         <is>
-          <t>2023-10-03</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D667" t="n">
-        <v>10000.05</v>
+        <v>75</v>
       </c>
       <c r="E667" t="n">
         <v>0</v>
@@ -37117,7 +37117,7 @@
         <v>0</v>
       </c>
       <c r="I667" t="n">
-        <v>10000.05</v>
+        <v>0</v>
       </c>
       <c r="J667" t="n">
         <v>0</v>
@@ -37129,35 +37129,35 @@
         <v>0</v>
       </c>
       <c r="M667" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="N667" t="n">
-        <v>10000.05</v>
+        <v>75</v>
       </c>
       <c r="O667" t="inlineStr">
         <is>
-          <t xml:space="preserve">149 </t>
+          <t xml:space="preserve">234 </t>
         </is>
       </c>
     </row>
     <row r="668">
       <c r="A668" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B668" t="inlineStr">
         <is>
-          <t>SB/01663</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C668" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D668" t="n">
-        <v>10000.05</v>
+        <v>385.5</v>
       </c>
       <c r="E668" t="n">
         <v>0</v>
@@ -37169,7 +37169,7 @@
         <v>0</v>
       </c>
       <c r="H668" t="n">
-        <v>10000.05</v>
+        <v>0</v>
       </c>
       <c r="I668" t="n">
         <v>0</v>
@@ -37184,14 +37184,14 @@
         <v>0</v>
       </c>
       <c r="M668" t="n">
-        <v>0</v>
+        <v>385.5</v>
       </c>
       <c r="N668" t="n">
-        <v>10000.05</v>
+        <v>385.5</v>
       </c>
       <c r="O668" t="inlineStr">
         <is>
-          <t xml:space="preserve">149 </t>
+          <t xml:space="preserve">L-000057 </t>
         </is>
       </c>
     </row>
@@ -37203,16 +37203,16 @@
       </c>
       <c r="B669" t="inlineStr">
         <is>
-          <t>SB/00441</t>
+          <t>SB/01194</t>
         </is>
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>2023-08-09</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="D669" t="n">
-        <v>3955</v>
+        <v>4263.26</v>
       </c>
       <c r="E669" t="n">
         <v>0</v>
@@ -37230,44 +37230,44 @@
         <v>0</v>
       </c>
       <c r="J669" t="n">
-        <v>0</v>
+        <v>4263.26</v>
       </c>
       <c r="K669" t="n">
         <v>0</v>
       </c>
       <c r="L669" t="n">
-        <v>3955</v>
+        <v>0</v>
       </c>
       <c r="M669" t="n">
         <v>0</v>
       </c>
       <c r="N669" t="n">
-        <v>3955</v>
+        <v>4263.26</v>
       </c>
       <c r="O669" t="inlineStr">
         <is>
-          <t xml:space="preserve">2338 </t>
+          <t xml:space="preserve">2478 </t>
         </is>
       </c>
     </row>
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/01147</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-09-17</t>
         </is>
       </c>
       <c r="D670" t="n">
-        <v>75</v>
+        <v>3390</v>
       </c>
       <c r="E670" t="n">
         <v>0</v>
@@ -37285,7 +37285,7 @@
         <v>0</v>
       </c>
       <c r="J670" t="n">
-        <v>0</v>
+        <v>3390</v>
       </c>
       <c r="K670" t="n">
         <v>0</v>
@@ -37294,14 +37294,14 @@
         <v>0</v>
       </c>
       <c r="M670" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="N670" t="n">
-        <v>75</v>
+        <v>3390</v>
       </c>
       <c r="O670" t="inlineStr">
         <is>
-          <t xml:space="preserve">234 </t>
+          <t xml:space="preserve">2475 </t>
         </is>
       </c>
     </row>
@@ -37322,7 +37322,7 @@
         </is>
       </c>
       <c r="D671" t="n">
-        <v>385.5</v>
+        <v>0.25</v>
       </c>
       <c r="E671" t="n">
         <v>0</v>
@@ -37349,35 +37349,35 @@
         <v>0</v>
       </c>
       <c r="M671" t="n">
-        <v>385.5</v>
+        <v>-0.25</v>
       </c>
       <c r="N671" t="n">
-        <v>385.5</v>
+        <v>-0.25</v>
       </c>
       <c r="O671" t="inlineStr">
         <is>
-          <t xml:space="preserve">L-000057 </t>
+          <t xml:space="preserve">1579 </t>
         </is>
       </c>
     </row>
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B672" t="inlineStr">
         <is>
-          <t>SB/01194</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C672" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D672" t="n">
-        <v>4263.26</v>
+        <v>1512</v>
       </c>
       <c r="E672" t="n">
         <v>0</v>
@@ -37395,7 +37395,7 @@
         <v>0</v>
       </c>
       <c r="J672" t="n">
-        <v>4263.26</v>
+        <v>0</v>
       </c>
       <c r="K672" t="n">
         <v>0</v>
@@ -37404,14 +37404,14 @@
         <v>0</v>
       </c>
       <c r="M672" t="n">
-        <v>0</v>
+        <v>1512</v>
       </c>
       <c r="N672" t="n">
-        <v>4263.26</v>
+        <v>1512</v>
       </c>
       <c r="O672" t="inlineStr">
         <is>
-          <t xml:space="preserve">2478 </t>
+          <t xml:space="preserve">530 </t>
         </is>
       </c>
     </row>
@@ -37423,16 +37423,16 @@
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>SB/01147</t>
+          <t>SB/00202</t>
         </is>
       </c>
       <c r="C673" t="inlineStr">
         <is>
-          <t>2023-09-17</t>
+          <t>2023-07-27</t>
         </is>
       </c>
       <c r="D673" t="n">
-        <v>3390</v>
+        <v>47460</v>
       </c>
       <c r="E673" t="n">
         <v>0</v>
@@ -37450,7 +37450,7 @@
         <v>0</v>
       </c>
       <c r="J673" t="n">
-        <v>3390</v>
+        <v>0</v>
       </c>
       <c r="K673" t="n">
         <v>0</v>
@@ -37459,14 +37459,14 @@
         <v>0</v>
       </c>
       <c r="M673" t="n">
-        <v>0</v>
+        <v>47460</v>
       </c>
       <c r="N673" t="n">
-        <v>3390</v>
+        <v>47460</v>
       </c>
       <c r="O673" t="inlineStr">
         <is>
-          <t xml:space="preserve">2475 </t>
+          <t xml:space="preserve">530 </t>
         </is>
       </c>
     </row>
@@ -37487,7 +37487,7 @@
         </is>
       </c>
       <c r="D674" t="n">
-        <v>0.25</v>
+        <v>22.6</v>
       </c>
       <c r="E674" t="n">
         <v>0</v>
@@ -37514,14 +37514,14 @@
         <v>0</v>
       </c>
       <c r="M674" t="n">
-        <v>-0.25</v>
+        <v>-22.6</v>
       </c>
       <c r="N674" t="n">
-        <v>-0.25</v>
+        <v>-22.6</v>
       </c>
       <c r="O674" t="inlineStr">
         <is>
-          <t xml:space="preserve">1579 </t>
+          <t xml:space="preserve">1928 </t>
         </is>
       </c>
     </row>
@@ -37542,7 +37542,7 @@
         </is>
       </c>
       <c r="D675" t="n">
-        <v>1512</v>
+        <v>352.5</v>
       </c>
       <c r="E675" t="n">
         <v>0</v>
@@ -37569,14 +37569,14 @@
         <v>0</v>
       </c>
       <c r="M675" t="n">
-        <v>1512</v>
+        <v>352.5</v>
       </c>
       <c r="N675" t="n">
-        <v>1512</v>
+        <v>352.5</v>
       </c>
       <c r="O675" t="inlineStr">
         <is>
-          <t xml:space="preserve">530 </t>
+          <t xml:space="preserve">1387 </t>
         </is>
       </c>
     </row>
@@ -37588,16 +37588,16 @@
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>SB/00202</t>
+          <t>SB/00419</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>2023-08-08</t>
         </is>
       </c>
       <c r="D676" t="n">
-        <v>47460</v>
+        <v>1130</v>
       </c>
       <c r="E676" t="n">
         <v>0</v>
@@ -37621,38 +37621,38 @@
         <v>0</v>
       </c>
       <c r="L676" t="n">
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="M676" t="n">
-        <v>47460</v>
+        <v>0</v>
       </c>
       <c r="N676" t="n">
-        <v>47460</v>
+        <v>1130</v>
       </c>
       <c r="O676" t="inlineStr">
         <is>
-          <t xml:space="preserve">530 </t>
+          <t xml:space="preserve">2140 </t>
         </is>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00684</t>
         </is>
       </c>
       <c r="C677" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-21</t>
         </is>
       </c>
       <c r="D677" t="n">
-        <v>22.6</v>
+        <v>440.7</v>
       </c>
       <c r="E677" t="n">
         <v>0</v>
@@ -37676,38 +37676,38 @@
         <v>0</v>
       </c>
       <c r="L677" t="n">
-        <v>0</v>
+        <v>440.7</v>
       </c>
       <c r="M677" t="n">
-        <v>-22.6</v>
+        <v>0</v>
       </c>
       <c r="N677" t="n">
-        <v>-22.6</v>
+        <v>440.7</v>
       </c>
       <c r="O677" t="inlineStr">
         <is>
-          <t xml:space="preserve">1928 </t>
+          <t xml:space="preserve">2140 </t>
         </is>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B678" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00802</t>
         </is>
       </c>
       <c r="C678" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-27</t>
         </is>
       </c>
       <c r="D678" t="n">
-        <v>352.5</v>
+        <v>9944</v>
       </c>
       <c r="E678" t="n">
         <v>0</v>
@@ -37728,20 +37728,20 @@
         <v>0</v>
       </c>
       <c r="K678" t="n">
-        <v>0</v>
+        <v>9944</v>
       </c>
       <c r="L678" t="n">
         <v>0</v>
       </c>
       <c r="M678" t="n">
-        <v>352.5</v>
+        <v>0</v>
       </c>
       <c r="N678" t="n">
-        <v>352.5</v>
+        <v>9944</v>
       </c>
       <c r="O678" t="inlineStr">
         <is>
-          <t xml:space="preserve">1387 </t>
+          <t xml:space="preserve">2140 </t>
         </is>
       </c>
     </row>
@@ -37753,16 +37753,16 @@
       </c>
       <c r="B679" t="inlineStr">
         <is>
-          <t>SB/00419</t>
+          <t>SB/00740</t>
         </is>
       </c>
       <c r="C679" t="inlineStr">
         <is>
-          <t>2023-08-08</t>
+          <t>2023-08-23</t>
         </is>
       </c>
       <c r="D679" t="n">
-        <v>1130</v>
+        <v>1594.66</v>
       </c>
       <c r="E679" t="n">
         <v>0</v>
@@ -37783,41 +37783,41 @@
         <v>0</v>
       </c>
       <c r="K679" t="n">
-        <v>0</v>
+        <v>1594.66</v>
       </c>
       <c r="L679" t="n">
-        <v>1130</v>
+        <v>0</v>
       </c>
       <c r="M679" t="n">
         <v>0</v>
       </c>
       <c r="N679" t="n">
-        <v>1130</v>
+        <v>1594.66</v>
       </c>
       <c r="O679" t="inlineStr">
         <is>
-          <t xml:space="preserve">2140 </t>
+          <t xml:space="preserve">997 </t>
         </is>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B680" t="inlineStr">
         <is>
-          <t>SB/00684</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C680" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D680" t="n">
-        <v>440.7</v>
+        <v>691</v>
       </c>
       <c r="E680" t="n">
         <v>0</v>
@@ -37841,17 +37841,17 @@
         <v>0</v>
       </c>
       <c r="L680" t="n">
-        <v>440.7</v>
+        <v>0</v>
       </c>
       <c r="M680" t="n">
-        <v>0</v>
+        <v>691</v>
       </c>
       <c r="N680" t="n">
-        <v>440.7</v>
+        <v>691</v>
       </c>
       <c r="O680" t="inlineStr">
         <is>
-          <t xml:space="preserve">2140 </t>
+          <t xml:space="preserve">942 </t>
         </is>
       </c>
     </row>
@@ -37863,16 +37863,16 @@
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>SB/00802</t>
+          <t>SB/01561</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>2023-08-27</t>
+          <t>2023-10-05</t>
         </is>
       </c>
       <c r="D681" t="n">
-        <v>9944</v>
+        <v>16385</v>
       </c>
       <c r="E681" t="n">
         <v>0</v>
@@ -37887,13 +37887,13 @@
         <v>0</v>
       </c>
       <c r="I681" t="n">
-        <v>0</v>
+        <v>16385</v>
       </c>
       <c r="J681" t="n">
         <v>0</v>
       </c>
       <c r="K681" t="n">
-        <v>9944</v>
+        <v>0</v>
       </c>
       <c r="L681" t="n">
         <v>0</v>
@@ -37902,32 +37902,32 @@
         <v>0</v>
       </c>
       <c r="N681" t="n">
-        <v>9944</v>
+        <v>16385</v>
       </c>
       <c r="O681" t="inlineStr">
         <is>
-          <t xml:space="preserve">2140 </t>
+          <t xml:space="preserve">942 </t>
         </is>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>SB/00740</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C682" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D682" t="n">
-        <v>1594.66</v>
+        <v>3111.29</v>
       </c>
       <c r="E682" t="n">
         <v>0</v>
@@ -37948,20 +37948,20 @@
         <v>0</v>
       </c>
       <c r="K682" t="n">
-        <v>1594.66</v>
+        <v>0</v>
       </c>
       <c r="L682" t="n">
         <v>0</v>
       </c>
       <c r="M682" t="n">
-        <v>0</v>
+        <v>3111.29</v>
       </c>
       <c r="N682" t="n">
-        <v>1594.66</v>
+        <v>3111.29</v>
       </c>
       <c r="O682" t="inlineStr">
         <is>
-          <t xml:space="preserve">997 </t>
+          <t xml:space="preserve">1447 </t>
         </is>
       </c>
     </row>
@@ -37982,7 +37982,7 @@
         </is>
       </c>
       <c r="D683" t="n">
-        <v>691</v>
+        <v>0.13</v>
       </c>
       <c r="E683" t="n">
         <v>0</v>
@@ -38009,35 +38009,35 @@
         <v>0</v>
       </c>
       <c r="M683" t="n">
-        <v>691</v>
+        <v>0.13</v>
       </c>
       <c r="N683" t="n">
-        <v>691</v>
+        <v>0.13</v>
       </c>
       <c r="O683" t="inlineStr">
         <is>
-          <t xml:space="preserve">942 </t>
+          <t xml:space="preserve">1608 </t>
         </is>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="inlineStr">
         <is>
-          <t>SB</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B684" t="inlineStr">
         <is>
-          <t>SB/01561</t>
+          <t>CO-&gt;CO-0000001</t>
         </is>
       </c>
       <c r="C684" t="inlineStr">
         <is>
-          <t>2023-10-05</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="D684" t="n">
-        <v>16385</v>
+        <v>20000.82</v>
       </c>
       <c r="E684" t="n">
         <v>0</v>
@@ -38052,7 +38052,7 @@
         <v>0</v>
       </c>
       <c r="I684" t="n">
-        <v>16385</v>
+        <v>0</v>
       </c>
       <c r="J684" t="n">
         <v>0</v>
@@ -38064,35 +38064,35 @@
         <v>0</v>
       </c>
       <c r="M684" t="n">
-        <v>0</v>
+        <v>20000.82</v>
       </c>
       <c r="N684" t="n">
-        <v>16385</v>
+        <v>20000.82</v>
       </c>
       <c r="O684" t="inlineStr">
         <is>
-          <t xml:space="preserve">942 </t>
+          <t xml:space="preserve">L-000058 </t>
         </is>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B685" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00177</t>
         </is>
       </c>
       <c r="C685" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="D685" t="n">
-        <v>3111.29</v>
+        <v>76840</v>
       </c>
       <c r="E685" t="n">
         <v>0</v>
@@ -38119,35 +38119,35 @@
         <v>0</v>
       </c>
       <c r="M685" t="n">
-        <v>3111.29</v>
+        <v>76840</v>
       </c>
       <c r="N685" t="n">
-        <v>3111.29</v>
+        <v>76840</v>
       </c>
       <c r="O685" t="inlineStr">
         <is>
-          <t xml:space="preserve">1447 </t>
+          <t xml:space="preserve">L-000058 </t>
         </is>
       </c>
     </row>
     <row r="686">
       <c r="A686" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00532</t>
         </is>
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-08-15</t>
         </is>
       </c>
       <c r="D686" t="n">
-        <v>0.13</v>
+        <v>38420</v>
       </c>
       <c r="E686" t="n">
         <v>0</v>
@@ -38171,38 +38171,38 @@
         <v>0</v>
       </c>
       <c r="L686" t="n">
-        <v>0</v>
+        <v>38420</v>
       </c>
       <c r="M686" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="N686" t="n">
-        <v>0.13</v>
+        <v>38420</v>
       </c>
       <c r="O686" t="inlineStr">
         <is>
-          <t xml:space="preserve">1608 </t>
+          <t xml:space="preserve">L-000058 </t>
         </is>
       </c>
     </row>
     <row r="687">
       <c r="A687" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>SB</t>
         </is>
       </c>
       <c r="B687" t="inlineStr">
         <is>
-          <t>CO-&gt;CO-0000001</t>
+          <t>SB/00919</t>
         </is>
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-09-05</t>
         </is>
       </c>
       <c r="D687" t="n">
-        <v>23680.82</v>
+        <v>76840</v>
       </c>
       <c r="E687" t="n">
         <v>0</v>
@@ -38223,16 +38223,16 @@
         <v>0</v>
       </c>
       <c r="K687" t="n">
-        <v>0</v>
+        <v>76840</v>
       </c>
       <c r="L687" t="n">
         <v>0</v>
       </c>
       <c r="M687" t="n">
-        <v>23680.82</v>
+        <v>0</v>
       </c>
       <c r="N687" t="n">
-        <v>23680.82</v>
+        <v>76840</v>
       </c>
       <c r="O687" t="inlineStr">
         <is>
@@ -38248,16 +38248,16 @@
       </c>
       <c r="B688" t="inlineStr">
         <is>
-          <t>SB/00177</t>
+          <t>SB/01544</t>
         </is>
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>2023-07-26</t>
+          <t>2023-10-04</t>
         </is>
       </c>
       <c r="D688" t="n">
-        <v>76840</v>
+        <v>134470</v>
       </c>
       <c r="E688" t="n">
         <v>0</v>
@@ -38272,7 +38272,7 @@
         <v>0</v>
       </c>
       <c r="I688" t="n">
-        <v>0</v>
+        <v>134470</v>
       </c>
       <c r="J688" t="n">
         <v>0</v>
@@ -38284,10 +38284,10 @@
         <v>0</v>
       </c>
       <c r="M688" t="n">
-        <v>76840</v>
+        <v>0</v>
       </c>
       <c r="N688" t="n">
-        <v>76840</v>
+        <v>134470</v>
       </c>
       <c r="O688" t="inlineStr">
         <is>
@@ -38303,16 +38303,16 @@
       </c>
       <c r="B689" t="inlineStr">
         <is>
-          <t>SB/00532</t>
+          <t>SB/01938</t>
         </is>
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>2023-08-15</t>
+          <t>2023-10-29</t>
         </is>
       </c>
       <c r="D689" t="n">
-        <v>38420</v>
+        <v>76840</v>
       </c>
       <c r="E689" t="n">
         <v>0</v>
@@ -38321,7 +38321,7 @@
         <v>0</v>
       </c>
       <c r="G689" t="n">
-        <v>0</v>
+        <v>76840</v>
       </c>
       <c r="H689" t="n">
         <v>0</v>
@@ -38336,13 +38336,13 @@
         <v>0</v>
       </c>
       <c r="L689" t="n">
-        <v>38420</v>
+        <v>0</v>
       </c>
       <c r="M689" t="n">
         <v>0</v>
       </c>
       <c r="N689" t="n">
-        <v>38420</v>
+        <v>76840</v>
       </c>
       <c r="O689" t="inlineStr">
         <is>
@@ -38358,12 +38358,12 @@
       </c>
       <c r="B690" t="inlineStr">
         <is>
-          <t>SB/00919</t>
+          <t>SB/02099</t>
         </is>
       </c>
       <c r="C690" t="inlineStr">
         <is>
-          <t>2023-09-05</t>
+          <t>2023-11-05</t>
         </is>
       </c>
       <c r="D690" t="n">
@@ -38376,7 +38376,7 @@
         <v>0</v>
       </c>
       <c r="G690" t="n">
-        <v>0</v>
+        <v>76840</v>
       </c>
       <c r="H690" t="n">
         <v>0</v>
@@ -38388,7 +38388,7 @@
         <v>0</v>
       </c>
       <c r="K690" t="n">
-        <v>76840</v>
+        <v>0</v>
       </c>
       <c r="L690" t="n">
         <v>0</v>
@@ -38413,22 +38413,22 @@
       </c>
       <c r="B691" t="inlineStr">
         <is>
-          <t>SB/01544</t>
+          <t>SB/02157</t>
         </is>
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>2023-10-04</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D691" t="n">
-        <v>134470</v>
+        <v>76840</v>
       </c>
       <c r="E691" t="n">
         <v>0</v>
       </c>
       <c r="F691" t="n">
-        <v>0</v>
+        <v>76840</v>
       </c>
       <c r="G691" t="n">
         <v>0</v>
@@ -38437,7 +38437,7 @@
         <v>0</v>
       </c>
       <c r="I691" t="n">
-        <v>134470</v>
+        <v>0</v>
       </c>
       <c r="J691" t="n">
         <v>0</v>
@@ -38452,7 +38452,7 @@
         <v>0</v>
       </c>
       <c r="N691" t="n">
-        <v>134470</v>
+        <v>76840</v>
       </c>
       <c r="O691" t="inlineStr">
         <is>
@@ -38468,25 +38468,25 @@
       </c>
       <c r="B692" t="inlineStr">
         <is>
-          <t>SB/01938</t>
+          <t>SB/02186</t>
         </is>
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>2023-10-29</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D692" t="n">
-        <v>76840</v>
+        <v>153680</v>
       </c>
       <c r="E692" t="n">
         <v>0</v>
       </c>
       <c r="F692" t="n">
-        <v>0</v>
+        <v>153680</v>
       </c>
       <c r="G692" t="n">
-        <v>76840</v>
+        <v>0</v>
       </c>
       <c r="H692" t="n">
         <v>0</v>
@@ -38507,7 +38507,7 @@
         <v>0</v>
       </c>
       <c r="N692" t="n">
-        <v>76840</v>
+        <v>153680</v>
       </c>
       <c r="O692" t="inlineStr">
         <is>
@@ -38523,25 +38523,25 @@
       </c>
       <c r="B693" t="inlineStr">
         <is>
-          <t>SB/02099</t>
+          <t>SB/02266</t>
         </is>
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-19</t>
         </is>
       </c>
       <c r="D693" t="n">
-        <v>76840</v>
+        <v>153680</v>
       </c>
       <c r="E693" t="n">
         <v>0</v>
       </c>
       <c r="F693" t="n">
-        <v>0</v>
+        <v>153680</v>
       </c>
       <c r="G693" t="n">
-        <v>76840</v>
+        <v>0</v>
       </c>
       <c r="H693" t="n">
         <v>0</v>
@@ -38562,174 +38562,9 @@
         <v>0</v>
       </c>
       <c r="N693" t="n">
-        <v>76840</v>
+        <v>153680</v>
       </c>
       <c r="O693" t="inlineStr">
-        <is>
-          <t xml:space="preserve">L-000058 </t>
-        </is>
-      </c>
-    </row>
-    <row r="694">
-      <c r="A694" t="inlineStr">
-        <is>
-          <t>SB</t>
-        </is>
-      </c>
-      <c r="B694" t="inlineStr">
-        <is>
-          <t>SB/02157</t>
-        </is>
-      </c>
-      <c r="C694" t="inlineStr">
-        <is>
-          <t>2023-11-07</t>
-        </is>
-      </c>
-      <c r="D694" t="n">
-        <v>76840</v>
-      </c>
-      <c r="E694" t="n">
-        <v>0</v>
-      </c>
-      <c r="F694" t="n">
-        <v>76840</v>
-      </c>
-      <c r="G694" t="n">
-        <v>0</v>
-      </c>
-      <c r="H694" t="n">
-        <v>0</v>
-      </c>
-      <c r="I694" t="n">
-        <v>0</v>
-      </c>
-      <c r="J694" t="n">
-        <v>0</v>
-      </c>
-      <c r="K694" t="n">
-        <v>0</v>
-      </c>
-      <c r="L694" t="n">
-        <v>0</v>
-      </c>
-      <c r="M694" t="n">
-        <v>0</v>
-      </c>
-      <c r="N694" t="n">
-        <v>76840</v>
-      </c>
-      <c r="O694" t="inlineStr">
-        <is>
-          <t xml:space="preserve">L-000058 </t>
-        </is>
-      </c>
-    </row>
-    <row r="695">
-      <c r="A695" t="inlineStr">
-        <is>
-          <t>SB</t>
-        </is>
-      </c>
-      <c r="B695" t="inlineStr">
-        <is>
-          <t>SB/02186</t>
-        </is>
-      </c>
-      <c r="C695" t="inlineStr">
-        <is>
-          <t>2023-11-08</t>
-        </is>
-      </c>
-      <c r="D695" t="n">
-        <v>153680</v>
-      </c>
-      <c r="E695" t="n">
-        <v>0</v>
-      </c>
-      <c r="F695" t="n">
-        <v>153680</v>
-      </c>
-      <c r="G695" t="n">
-        <v>0</v>
-      </c>
-      <c r="H695" t="n">
-        <v>0</v>
-      </c>
-      <c r="I695" t="n">
-        <v>0</v>
-      </c>
-      <c r="J695" t="n">
-        <v>0</v>
-      </c>
-      <c r="K695" t="n">
-        <v>0</v>
-      </c>
-      <c r="L695" t="n">
-        <v>0</v>
-      </c>
-      <c r="M695" t="n">
-        <v>0</v>
-      </c>
-      <c r="N695" t="n">
-        <v>153680</v>
-      </c>
-      <c r="O695" t="inlineStr">
-        <is>
-          <t xml:space="preserve">L-000058 </t>
-        </is>
-      </c>
-    </row>
-    <row r="696">
-      <c r="A696" t="inlineStr">
-        <is>
-          <t>SB</t>
-        </is>
-      </c>
-      <c r="B696" t="inlineStr">
-        <is>
-          <t>SB/02266</t>
-        </is>
-      </c>
-      <c r="C696" t="inlineStr">
-        <is>
-          <t>2023-11-19</t>
-        </is>
-      </c>
-      <c r="D696" t="n">
-        <v>153680</v>
-      </c>
-      <c r="E696" t="n">
-        <v>0</v>
-      </c>
-      <c r="F696" t="n">
-        <v>153680</v>
-      </c>
-      <c r="G696" t="n">
-        <v>0</v>
-      </c>
-      <c r="H696" t="n">
-        <v>0</v>
-      </c>
-      <c r="I696" t="n">
-        <v>0</v>
-      </c>
-      <c r="J696" t="n">
-        <v>0</v>
-      </c>
-      <c r="K696" t="n">
-        <v>0</v>
-      </c>
-      <c r="L696" t="n">
-        <v>0</v>
-      </c>
-      <c r="M696" t="n">
-        <v>0</v>
-      </c>
-      <c r="N696" t="n">
-        <v>153680</v>
-      </c>
-      <c r="O696" t="inlineStr">
         <is>
           <t xml:space="preserve">L-000058 </t>
         </is>

</xml_diff>